<commit_message>
add leaf skeleton analysis
</commit_message>
<xml_diff>
--- a/sample_test/trait.xlsx
+++ b/sample_test/trait.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -388,7 +388,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/01</t>
+          <t>01.jpg</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -404,13 +404,13 @@
         <v>347</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02710754148128464</v>
+        <v>0.02431618966192055</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/02</t>
+          <t>02.jpg</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -426,13 +426,13 @@
         <v>434</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02315092530916385</v>
+        <v>0.02228918141274923</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/03</t>
+          <t>03.jpg</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -448,13 +448,13 @@
         <v>533</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0266610496858301</v>
+        <v>0.02637357401543597</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/04</t>
+          <t>04.jpg</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -476,7 +476,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/05</t>
+          <t>05.jpg</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -492,13 +492,13 @@
         <v>282</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03014249037894378</v>
+        <v>0.03033984992984335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/06</t>
+          <t>06.jpg</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -514,13 +514,13 @@
         <v>437</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02275953092975364</v>
+        <v>0.0223175500808994</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/07</t>
+          <t>07.jpg</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -536,13 +536,13 @@
         <v>345</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03251495997153989</v>
+        <v>0.03061937810892377</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/08</t>
+          <t>08.jpg</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -564,7 +564,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/09</t>
+          <t>09.jpg</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -586,7 +586,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/10</t>
+          <t>10.jpg</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -602,13 +602,13 @@
         <v>223</v>
       </c>
       <c r="F11" t="n">
-        <v>0.03531367418015233</v>
+        <v>0.03024929369681965</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/11</t>
+          <t>11.jpg</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -630,7 +630,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/12</t>
+          <t>12.jpg</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -646,13 +646,13 @@
         <v>130</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05368492946311532</v>
+        <v>0.04358519734800191</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/13</t>
+          <t>13.jpg</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -668,13 +668,13 @@
         <v>377</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02937228256611372</v>
+        <v>0.02889985840097764</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/14</t>
+          <t>14.jpg</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -696,7 +696,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/15</t>
+          <t>15.jpg</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -712,13 +712,13 @@
         <v>448</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02278927482147935</v>
+        <v>0.02277738808077557</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/16</t>
+          <t>16.jpg</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -734,13 +734,13 @@
         <v>457</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02177322148930879</v>
+        <v>0.021025794516685</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/17</t>
+          <t>17.jpg</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -756,13 +756,13 @@
         <v>404</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02194680716006768</v>
+        <v>0.02189514940431469</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/18</t>
+          <t>18.jpg</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -784,7 +784,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/19</t>
+          <t>19.jpg</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -806,7 +806,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/20</t>
+          <t>20.jpg</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -822,13 +822,13 @@
         <v>348</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02576886652606792</v>
+        <v>0.02408844832033849</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/21</t>
+          <t>21.jpg</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -850,7 +850,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/22</t>
+          <t>22.jpg</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -872,7 +872,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/23</t>
+          <t>23.jpg</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -894,7 +894,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/24</t>
+          <t>24.jpg</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -910,13 +910,13 @@
         <v>482</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0207220590622024</v>
+        <v>0.01952270447514764</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/25</t>
+          <t>25.jpg</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -938,7 +938,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/26</t>
+          <t>26.jpg</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -954,13 +954,13 @@
         <v>110</v>
       </c>
       <c r="F27" t="n">
-        <v>0.05472549135098805</v>
+        <v>0.04119880719597929</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/27</t>
+          <t>27.jpg</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -976,13 +976,13 @@
         <v>373</v>
       </c>
       <c r="F28" t="n">
-        <v>0.02594640172615418</v>
+        <v>0.02340937419056989</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/28</t>
+          <t>28.jpg</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1004,7 +1004,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/29</t>
+          <t>29.jpg</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1026,7 +1026,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/30</t>
+          <t>30.jpg</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1042,13 +1042,13 @@
         <v>281</v>
       </c>
       <c r="F31" t="n">
-        <v>0.03045462647900538</v>
+        <v>0.0304184855363709</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/31</t>
+          <t>31.jpg</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1070,7 +1070,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>/home/suxingliu/plant-image-analysis/sample_test/32</t>
+          <t>32.jpg</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1086,10 +1086,10 @@
         <v>282</v>
       </c>
       <c r="F33" t="n">
-        <v>0.04283078611107215</v>
+        <v>0.03572362339409182</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add invidual leaf segmentation module
</commit_message>
<xml_diff>
--- a/sample_test/trait.xlsx
+++ b/sample_test/trait.xlsx
@@ -727,10 +727,10 @@
         <v>271</v>
       </c>
       <c r="F12" t="n">
-        <v>0.03354666239055938</v>
+        <v>0.02627101832065298</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">

</xml_diff>